<commit_message>
Update 10/07/2023 : MED files + update "photo to take"
</commit_message>
<xml_diff>
--- a/data/matu_scale.xlsx
+++ b/data/matu_scale.xlsx
@@ -1061,7 +1061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E841"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A831" workbookViewId="0">
       <selection activeCell="D215" sqref="D215"/>
     </sheetView>
   </sheetViews>
@@ -15384,7 +15384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E835"/>
   <sheetViews>
-    <sheetView topLeftCell="A801" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView topLeftCell="A807" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="D476" sqref="D476"/>
     </sheetView>
   </sheetViews>

</xml_diff>